<commit_message>
Fixing README and INFO. Adding BoM
</commit_message>
<xml_diff>
--- a/SAMD51_Breakout_BoM.xlsx
+++ b/SAMD51_Breakout_BoM.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="173">
   <si>
     <t>Item</t>
   </si>
@@ -313,6 +313,234 @@
   </si>
   <si>
     <t>C5,C6</t>
+  </si>
+  <si>
+    <t>TERM BLOCK HDR 2POS 90DEG 3.5MM</t>
+  </si>
+  <si>
+    <t>277-2416-ND</t>
+  </si>
+  <si>
+    <t>Phoenix Contact</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 10POS 2.54MM</t>
+  </si>
+  <si>
+    <t>2057-PH1RB-10-UA-ND</t>
+  </si>
+  <si>
+    <t>Adam Tech</t>
+  </si>
+  <si>
+    <t>PH1RB-10-UA</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 24POS 2.54MM</t>
+  </si>
+  <si>
+    <t>S1131EC-24-ND</t>
+  </si>
+  <si>
+    <t>Sullins Connector Solutions</t>
+  </si>
+  <si>
+    <t>PRPC024SACN-RC</t>
+  </si>
+  <si>
+    <t>CONN RCPT USB2.0 MICRO B SMD R/A</t>
+  </si>
+  <si>
+    <t>609-4613-1-ND</t>
+  </si>
+  <si>
+    <t>Amphenol ICC (FCI)</t>
+  </si>
+  <si>
+    <t>10118192-0001LF</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 5V 1A SOT223</t>
+  </si>
+  <si>
+    <t>NCP1117ST50T3GOSCT-ND</t>
+  </si>
+  <si>
+    <t>ON Semiconductor</t>
+  </si>
+  <si>
+    <t>NCP1117ST50T3G</t>
+  </si>
+  <si>
+    <t>IC REG LINEAR 3.3V 1.2A SOT223</t>
+  </si>
+  <si>
+    <t>497-17239-1-ND</t>
+  </si>
+  <si>
+    <t>STMicroelectronics</t>
+  </si>
+  <si>
+    <t>LDL1117S33R</t>
+  </si>
+  <si>
+    <t>IC MCU 32BIT 1MB FLASH 64TQFP</t>
+  </si>
+  <si>
+    <t>ATSAMD51J20A-AU-ND</t>
+  </si>
+  <si>
+    <t>Microchip Technology</t>
+  </si>
+  <si>
+    <t>ATSAMD51J20A-AU</t>
+  </si>
+  <si>
+    <t>IC FLASH 4M SPI 104MHZ 8SOIC</t>
+  </si>
+  <si>
+    <t>W25X40CLSNIG-ND</t>
+  </si>
+  <si>
+    <t>Winbond Electronics</t>
+  </si>
+  <si>
+    <t>W25X40CLSNIG</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 40V 1A SOD123</t>
+  </si>
+  <si>
+    <t>1N5819HW-FDICT-ND</t>
+  </si>
+  <si>
+    <t>1N5819HW-7-F</t>
+  </si>
+  <si>
+    <t>LED GREEN DIFFUSED 0603 SMD</t>
+  </si>
+  <si>
+    <t>475-3118-1-ND</t>
+  </si>
+  <si>
+    <t>OSRAM Opto Semiconductors Inc.</t>
+  </si>
+  <si>
+    <t>LG L29K-F2J1-24-Z</t>
+  </si>
+  <si>
+    <t>CRYSTAL 32.768KHZ 12.5PF SMD</t>
+  </si>
+  <si>
+    <t>2195-CM7V-T1A-32.768KHZ-12.5PF-20PPM-TA-QCCT-ND</t>
+  </si>
+  <si>
+    <t>Micro Crystal AG</t>
+  </si>
+  <si>
+    <t>CM7V-T1A-32.768KHZ-12.5PF-20PPM-TA-QC</t>
+  </si>
+  <si>
+    <t>TACT 4.5 X 4.5, 3.8 MM H, 2.5N,</t>
+  </si>
+  <si>
+    <t>PTS647SK38SMTR2LFSCT-ND</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>PTS 647 SK38 SMTR2 LFS</t>
+  </si>
+  <si>
+    <t>FIXED IND 10UH 150MA 360 MOHM</t>
+  </si>
+  <si>
+    <t>587-2045-1-ND</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>LBR2012T100K</t>
+  </si>
+  <si>
+    <t>CAP CER 22UF 25V X5R 0805</t>
+  </si>
+  <si>
+    <t>1276-2908-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CL21A226MAQNNNE</t>
+  </si>
+  <si>
+    <t>CAP CER 47UF 6.3V X5R 0805</t>
+  </si>
+  <si>
+    <t>490-9960-1-ND</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>GRM21BR60J476ME15L</t>
+  </si>
+  <si>
+    <t>CAP CER 15PF 50V C0G/NPO 0402</t>
+  </si>
+  <si>
+    <t>311-1642-1-ND</t>
+  </si>
+  <si>
+    <t>CC0402FRNPO9BN150</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 6.3V X5R 0805</t>
+  </si>
+  <si>
+    <t>1276-2405-1-ND</t>
+  </si>
+  <si>
+    <t>CL21A106KQCLRNC</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1UF 25V X7R 0603</t>
+  </si>
+  <si>
+    <t>311-1341-1-ND</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R8BB104</t>
+  </si>
+  <si>
+    <t>CAP CER 4.7UF 6.3V X5R 0603</t>
+  </si>
+  <si>
+    <t>1276-1045-1-ND</t>
+  </si>
+  <si>
+    <t>CL10A475KQ8NNNC</t>
+  </si>
+  <si>
+    <t>RES 820 OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>RMCF0805FT820RCT-ND</t>
+  </si>
+  <si>
+    <t>Stackpole Electronics Inc</t>
+  </si>
+  <si>
+    <t>RMCF0805FT820R</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>311-10.0KCRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0805FR-0710KL</t>
   </si>
 </sst>
 </file>
@@ -1269,10 +1497,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1362,21 +1590,31 @@
       <c r="B3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1844210</v>
+      </c>
       <c r="G3" s="3">
         <v>1</v>
       </c>
-      <c r="H3" s="6"/>
+      <c r="H3" s="6">
+        <v>1.42</v>
+      </c>
       <c r="I3" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.42</v>
       </c>
       <c r="J3" s="2" t="str">
         <f t="shared" ref="J3:J24" si="1">HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",D3))</f>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=277-2416-ND</v>
       </c>
     </row>
     <row r="4" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1386,21 +1624,31 @@
       <c r="B4" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11"/>
+      <c r="C4" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>103</v>
+      </c>
       <c r="G4" s="11">
         <v>1</v>
       </c>
-      <c r="H4" s="12"/>
+      <c r="H4" s="12">
+        <v>0.41</v>
+      </c>
       <c r="I4" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.41</v>
       </c>
       <c r="J4" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=2057-PH1RB-10-UA-ND</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1410,21 +1658,31 @@
       <c r="B5" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="3"/>
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>107</v>
+      </c>
       <c r="G5" s="3">
         <v>2</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="6">
+        <v>1.1000000000000001</v>
+      </c>
       <c r="I5" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="J5" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=S1131EC-24-ND</v>
       </c>
     </row>
     <row r="6" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1434,21 +1692,31 @@
       <c r="B6" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="11"/>
+      <c r="C6" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>111</v>
+      </c>
       <c r="G6" s="11">
         <v>1</v>
       </c>
-      <c r="H6" s="12"/>
+      <c r="H6" s="12">
+        <v>0.66</v>
+      </c>
       <c r="I6" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.66</v>
       </c>
       <c r="J6" s="12" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=609-4613-1-ND</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,21 +1726,31 @@
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="3"/>
+      <c r="C7" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>115</v>
+      </c>
       <c r="G7" s="3">
         <v>1</v>
       </c>
-      <c r="H7" s="6"/>
+      <c r="H7" s="6">
+        <v>0.76</v>
+      </c>
       <c r="I7" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.76</v>
       </c>
       <c r="J7" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=NCP1117ST50T3GOSCT-ND</v>
       </c>
     </row>
     <row r="8" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1482,21 +1760,31 @@
       <c r="B8" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="C8" s="10"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="11"/>
+      <c r="C8" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>119</v>
+      </c>
       <c r="G8" s="11">
         <v>1</v>
       </c>
-      <c r="H8" s="12"/>
+      <c r="H8" s="12">
+        <v>0.69</v>
+      </c>
       <c r="I8" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.69</v>
       </c>
       <c r="J8" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=497-17239-1-ND</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1506,21 +1794,31 @@
       <c r="B9" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="3"/>
+      <c r="C9" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>123</v>
+      </c>
       <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="6"/>
+      <c r="H9" s="6">
+        <v>7.89</v>
+      </c>
       <c r="I9" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.89</v>
       </c>
       <c r="J9" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=ATSAMD51J20A-AU-ND</v>
       </c>
     </row>
     <row r="10" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1530,21 +1828,31 @@
       <c r="B10" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C10" s="10"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
+      <c r="C10" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>127</v>
+      </c>
       <c r="G10" s="11">
         <v>1</v>
       </c>
-      <c r="H10" s="12"/>
+      <c r="H10" s="12">
+        <v>0.59</v>
+      </c>
       <c r="I10" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.59</v>
       </c>
       <c r="J10" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=W25X40CLSNIG-ND</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1554,21 +1862,31 @@
       <c r="B11" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
+      <c r="C11" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>130</v>
+      </c>
       <c r="G11" s="3">
         <v>2</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="6">
+        <v>0.61</v>
+      </c>
       <c r="I11" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.22</v>
       </c>
       <c r="J11" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=1N5819HW-FDICT-ND</v>
       </c>
     </row>
     <row r="12" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,21 +1896,31 @@
       <c r="B12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="11"/>
+      <c r="C12" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>134</v>
+      </c>
       <c r="G12" s="11">
         <v>4</v>
       </c>
-      <c r="H12" s="12"/>
+      <c r="H12" s="12">
+        <v>0.62</v>
+      </c>
       <c r="I12" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.48</v>
       </c>
       <c r="J12" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=475-3118-1-ND</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1602,21 +1930,31 @@
       <c r="B13" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="3"/>
+      <c r="C13" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>138</v>
+      </c>
       <c r="G13" s="3">
         <v>1</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="6">
+        <v>0.67</v>
+      </c>
       <c r="I13" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.67</v>
       </c>
       <c r="J13" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=2195-CM7V-T1A-32.768KHZ-12.5PF-20PPM-TA-QCCT-ND</v>
       </c>
     </row>
     <row r="14" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1626,21 +1964,31 @@
       <c r="B14" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="11"/>
+      <c r="C14" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>142</v>
+      </c>
       <c r="G14" s="11">
         <v>1</v>
       </c>
-      <c r="H14" s="12"/>
+      <c r="H14" s="12">
+        <v>0.23</v>
+      </c>
       <c r="I14" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.23</v>
       </c>
       <c r="J14" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=PTS647SK38SMTR2LFSCT-ND</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1650,21 +1998,31 @@
       <c r="B15" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C15" s="1"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="3"/>
+      <c r="C15" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>146</v>
+      </c>
       <c r="G15" s="3">
         <v>2</v>
       </c>
-      <c r="H15" s="6"/>
+      <c r="H15" s="6">
+        <v>0.21</v>
+      </c>
       <c r="I15" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="J15" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=587-2045-1-ND</v>
       </c>
     </row>
     <row r="16" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1674,21 +2032,31 @@
       <c r="B16" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="12"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="11"/>
+      <c r="C16" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>149</v>
+      </c>
       <c r="G16" s="11">
         <v>1</v>
       </c>
-      <c r="H16" s="12"/>
+      <c r="H16" s="12">
+        <v>0.8</v>
+      </c>
       <c r="I16" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J16" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=1276-2908-1-ND</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1698,21 +2066,31 @@
       <c r="B17" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="3"/>
+      <c r="C17" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>153</v>
+      </c>
       <c r="G17" s="3">
         <v>1</v>
       </c>
-      <c r="H17" s="6"/>
+      <c r="H17" s="6">
+        <v>0.8</v>
+      </c>
       <c r="I17" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J17" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=490-9960-1-ND</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1722,21 +2100,31 @@
       <c r="B18" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="11"/>
+      <c r="C18" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>156</v>
+      </c>
       <c r="G18" s="11">
         <v>2</v>
       </c>
-      <c r="H18" s="12"/>
+      <c r="H18" s="12">
+        <v>0.18</v>
+      </c>
       <c r="I18" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.36</v>
       </c>
       <c r="J18" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=311-1642-1-ND</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1746,21 +2134,31 @@
       <c r="B19" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="3"/>
+      <c r="C19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>159</v>
+      </c>
       <c r="G19" s="3">
         <v>2</v>
       </c>
-      <c r="H19" s="6"/>
+      <c r="H19" s="6">
+        <v>0.17</v>
+      </c>
       <c r="I19" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.34</v>
       </c>
       <c r="J19" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=1276-2405-1-ND</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1770,21 +2168,31 @@
       <c r="B20" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="11"/>
+      <c r="C20" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>162</v>
+      </c>
       <c r="G20" s="11">
         <v>6</v>
       </c>
-      <c r="H20" s="12"/>
+      <c r="H20" s="12">
+        <v>0.15</v>
+      </c>
       <c r="I20" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="J20" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=311-1341-1-ND</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1794,21 +2202,31 @@
       <c r="B21" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3"/>
+      <c r="C21" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>165</v>
+      </c>
       <c r="G21" s="3">
         <v>1</v>
       </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="6">
+        <v>0.15</v>
+      </c>
       <c r="I21" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="J21" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=1276-1045-1-ND</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1818,21 +2236,31 @@
       <c r="B22" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="12"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="11"/>
+      <c r="C22" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>169</v>
+      </c>
       <c r="G22" s="11">
         <v>5</v>
       </c>
-      <c r="H22" s="12"/>
+      <c r="H22" s="12">
+        <v>0.16</v>
+      </c>
       <c r="I22" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="J22" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=RMCF0805FT820RCT-ND</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1842,21 +2270,31 @@
       <c r="B23" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="C23" s="1"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="3"/>
+      <c r="C23" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>172</v>
+      </c>
       <c r="G23" s="3">
         <v>2</v>
       </c>
-      <c r="H23" s="6"/>
+      <c r="H23" s="6">
+        <v>0.16</v>
+      </c>
       <c r="I23" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="J23" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>https://www.digikey.com/products/en?keywords=311-10.0KCRCT-ND</v>
       </c>
     </row>
     <row r="24" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1892,87 +2330,7 @@
       </c>
       <c r="I25" s="2">
         <f>SUM(I2:I24)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="10">
-        <v>14</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="10">
-        <f t="shared" ref="I36:I39" si="2">H36*G36</f>
-        <v>0</v>
-      </c>
-      <c r="J36" s="10" t="str">
-        <f t="shared" ref="J36:J39" si="3">HYPERLINK(CONCATENATE("https://www.digikey.com/products/en?keywords=",D36))</f>
-        <v>https://www.digikey.com/products/en?keywords=</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>15</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" s="13" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10">
-        <v>16</v>
-      </c>
-      <c r="B38" s="10"/>
-      <c r="C38" s="10"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="10" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>17</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="J39" s="2" t="str">
-        <f t="shared" si="3"/>
-        <v>https://www.digikey.com/products/en?keywords=</v>
+        <v>29.110000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>